<commit_message>
Update ENA run accessions after data upload
</commit_message>
<xml_diff>
--- a/06-figures_tables/Dataset_S1.xlsx
+++ b/06-figures_tables/Dataset_S1.xlsx
@@ -1741,7 +1741,7 @@
     <t>ERR3579704</t>
   </si>
   <si>
-    <t>ERRX000004</t>
+    <t>ERR10114847</t>
   </si>
   <si>
     <t>ERR3579707</t>
@@ -1762,13 +1762,13 @@
     <t>ERR3579730</t>
   </si>
   <si>
-    <t>ERRX000031</t>
+    <t>ERR10114848</t>
   </si>
   <si>
     <t>ERR3579731</t>
   </si>
   <si>
-    <t>ERRX000034</t>
+    <t>ERR10114849</t>
   </si>
   <si>
     <t>ERR3579732</t>
@@ -1783,7 +1783,7 @@
     <t>ERR3579735</t>
   </si>
   <si>
-    <t>ERRX000040</t>
+    <t>ERR10114850</t>
   </si>
   <si>
     <t>ERR3579736</t>
@@ -1810,16 +1810,16 @@
     <t>ERR3579745</t>
   </si>
   <si>
-    <t>ERRX000051</t>
+    <t>ERR10114851</t>
   </si>
   <si>
     <t>ERR3579746</t>
   </si>
   <si>
-    <t>ERRX000053</t>
-  </si>
-  <si>
-    <t>ERRX000054</t>
+    <t>ERR10114852</t>
+  </si>
+  <si>
+    <t>ERR10114844</t>
   </si>
   <si>
     <t>ERR3579747</t>
@@ -1828,7 +1828,7 @@
     <t>ERR3579748</t>
   </si>
   <si>
-    <t>ERRX000057</t>
+    <t>ERR10114853</t>
   </si>
   <si>
     <t>ERR3579673</t>
@@ -1837,22 +1837,22 @@
     <t>ERR3678727</t>
   </si>
   <si>
-    <t>ERRX000068</t>
+    <t>ERR10114854</t>
   </si>
   <si>
     <t>ERR3579674</t>
   </si>
   <si>
-    <t>ERRX000070</t>
-  </si>
-  <si>
-    <t>ERRX000071</t>
+    <t>ERR10114855</t>
+  </si>
+  <si>
+    <t>ERR10114845</t>
   </si>
   <si>
     <t>ERR3579754</t>
   </si>
   <si>
-    <t>ERRX000073</t>
+    <t>ERR10114856</t>
   </si>
   <si>
     <t>ERR3307045</t>
@@ -1930,16 +1930,16 @@
     <t>ERR3579791</t>
   </si>
   <si>
-    <t>ERRX000150</t>
+    <t>ERR10114857</t>
   </si>
   <si>
     <t>ERR3579688</t>
   </si>
   <si>
-    <t>ERRX000160</t>
-  </si>
-  <si>
-    <t>ERRX000161</t>
+    <t>ERR10114858</t>
+  </si>
+  <si>
+    <t>ERR10114846</t>
   </si>
   <si>
     <t>ERR3678187</t>
@@ -1948,7 +1948,7 @@
     <t>ERR3579800</t>
   </si>
   <si>
-    <t>ERRX000164</t>
+    <t>ERR10114859</t>
   </si>
   <si>
     <t>ERR3579801</t>
@@ -1969,22 +1969,22 @@
     <t>ERR3579806</t>
   </si>
   <si>
-    <t>ERRX000171</t>
+    <t>ERR10114860</t>
   </si>
   <si>
     <t>ERR3579807</t>
   </si>
   <si>
-    <t>ERRX000173</t>
+    <t>ERR10114861</t>
   </si>
   <si>
     <t>ERR3579808</t>
   </si>
   <si>
-    <t>ERRX000175</t>
-  </si>
-  <si>
-    <t>ERRX000176</t>
+    <t>ERR10114862</t>
+  </si>
+  <si>
+    <t>ERR10114863</t>
   </si>
   <si>
     <t>ERR3579809</t>
@@ -2038,16 +2038,16 @@
     <t>ERR3579827</t>
   </si>
   <si>
-    <t>ERRX000197</t>
+    <t>ERR10114864</t>
   </si>
   <si>
     <t>ERR3579830</t>
   </si>
   <si>
-    <t>ERRX000200</t>
-  </si>
-  <si>
-    <t>ERRX000201</t>
+    <t>ERR10114865</t>
+  </si>
+  <si>
+    <t>ERR10114866</t>
   </si>
   <si>
     <t>Fellows Yates et al. (2021)</t>

</xml_diff>